<commit_message>
Web element initial commit
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Automation\ABS-CBN_DotCom_Web_Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABS-CBN_Push_Automation\ABS-CBN_IMP_PUSH_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="5688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="5685"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -359,16 +359,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -376,7 +376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -384,7 +384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1052023</v>
       </c>

</xml_diff>